<commit_message>
Updated results for ex. 3 hw4
</commit_message>
<xml_diff>
--- a/hw4/dbsys-hw4/Results.xlsx
+++ b/hw4/dbsys-hw4/Results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="25">
   <si>
     <t>Exercise 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,6 +92,38 @@
   </si>
   <si>
     <t>Exercise 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimized</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Out-of-the-box</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -173,7 +206,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -184,6 +217,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -356,11 +392,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="374873440"/>
-        <c:axId val="374874224"/>
+        <c:axId val="317910072"/>
+        <c:axId val="319762168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374873440"/>
+        <c:axId val="317910072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -403,7 +439,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374874224"/>
+        <c:crossAx val="319762168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -411,7 +447,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374874224"/>
+        <c:axId val="319762168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,7 +554,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374873440"/>
+        <c:crossAx val="317910072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -718,11 +754,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="379942728"/>
-        <c:axId val="379951352"/>
+        <c:axId val="319762952"/>
+        <c:axId val="319759424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379942728"/>
+        <c:axId val="319762952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -765,7 +801,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379951352"/>
+        <c:crossAx val="319759424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -773,7 +809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379951352"/>
+        <c:axId val="319759424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +921,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379942728"/>
+        <c:crossAx val="319762952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1081,11 +1117,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="379946256"/>
-        <c:axId val="379941944"/>
+        <c:axId val="319761776"/>
+        <c:axId val="319761384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379946256"/>
+        <c:axId val="319761776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1164,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379941944"/>
+        <c:crossAx val="319761384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1136,7 +1172,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379941944"/>
+        <c:axId val="319761384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,7 +1284,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379946256"/>
+        <c:crossAx val="319761776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1444,11 +1480,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="373513608"/>
-        <c:axId val="373515176"/>
+        <c:axId val="319757464"/>
+        <c:axId val="319757856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="373513608"/>
+        <c:axId val="319757464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,7 +1527,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373515176"/>
+        <c:crossAx val="319757856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1499,7 +1535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373515176"/>
+        <c:axId val="319757856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1606,7 +1642,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373513608"/>
+        <c:crossAx val="319757464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1802,11 +1838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="379943904"/>
-        <c:axId val="379942336"/>
+        <c:axId val="319758248"/>
+        <c:axId val="319758640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="379943904"/>
+        <c:axId val="319758248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1885,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379942336"/>
+        <c:crossAx val="319758640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1857,7 +1893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="379942336"/>
+        <c:axId val="319758640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,7 +2000,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379943904"/>
+        <c:crossAx val="319758248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2160,11 +2196,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="319683000"/>
-        <c:axId val="319683392"/>
+        <c:axId val="319760992"/>
+        <c:axId val="319890352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319683000"/>
+        <c:axId val="319760992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,7 +2243,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319683392"/>
+        <c:crossAx val="319890352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2215,7 +2251,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319683392"/>
+        <c:axId val="319890352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2322,7 +2358,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319683000"/>
+        <c:crossAx val="319760992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2518,11 +2554,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="447995592"/>
-        <c:axId val="447996376"/>
+        <c:axId val="319893880"/>
+        <c:axId val="319889568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="447995592"/>
+        <c:axId val="319893880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2601,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="447996376"/>
+        <c:crossAx val="319889568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2573,7 +2609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="447996376"/>
+        <c:axId val="319889568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2680,7 +2716,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="447995592"/>
+        <c:crossAx val="319893880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2820,53 +2856,111 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$64:$A$69</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Query 1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Query 3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Query 5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Query 6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Query 18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Query 22</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet2!$A$1:$B$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Out-of-the-box</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Optimized</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Q5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Q6</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Q18</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Q22</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$64:$G$69</c:f>
+              <c:f>Sheet2!$C$1:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>5.1339999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1.24</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>1.9439999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.42799999999999994</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>2.4739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6.5999999999999989E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
+                  <c:v>1.046</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
+                  <c:v>3.6680000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.27800000000000002</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="10">
+                  <c:v>0.41600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2882,11 +2976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="447983832"/>
-        <c:axId val="447985400"/>
+        <c:axId val="342265808"/>
+        <c:axId val="342257968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="447983832"/>
+        <c:axId val="342265808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2929,7 +3023,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="447985400"/>
+        <c:crossAx val="342257968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2937,7 +3031,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="447985400"/>
+        <c:axId val="342257968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,8 +3072,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" altLang="ko-KR"/>
-                  <a:t>Average Elapsed Time (sec.)</a:t>
+                  <a:t>Average Elapsed</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="ko-KR" baseline="0"/>
+                  <a:t> Time (sec.)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" altLang="ko-KR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3044,7 +3143,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="447983832"/>
+        <c:crossAx val="342265808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7665,22 +7764,27 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>15875</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>612775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>82</xdr:row>
-      <xdr:rowOff>168275</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7689,7 +7793,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7963,8 +8067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -9162,4 +9266,152 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1">
+        <v>5.1339999999999995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4"/>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>1.9439999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="4"/>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0.42799999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>2.4739999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>6.5999999999999989E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1.046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>3.6680000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4"/>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>0.41600000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="4"/>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>